<commit_message>
fix: expected result type convert
</commit_message>
<xml_diff>
--- a/backend/resources/test.xlsx
+++ b/backend/resources/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\课程\SoftwareTesting_杜庆峰\course_project\TJ_2025Spring_SoftwareTesting_TestingTool\backend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914B6F46-4E0B-4FF7-B0C5-5CF725C77B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DF0679-0466-42AC-ACD7-948516093337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,10 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{'plot_count': 0, 'plant_plot_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0], 'plant_disease_count': {}, 'disease_count': {}, 'prediction': 'mocked_prediction'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[{
     'plotId': 'p1',
     'plotName': '地块1',
@@ -110,12 +106,36 @@
     <t>list(schemas.form.PlotDetails)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>{'disease_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0], 'plant_disease_count': {}, 'plant_plot_count': {'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>植物</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A': 1}, 'plot_count': 1, 'prediction': 'p'}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +155,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -446,12 +473,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.58203125" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
@@ -498,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
@@ -506,19 +533,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
@@ -538,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
@@ -558,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: homework seller bonus and add excel
</commit_message>
<xml_diff>
--- a/backend/resources/test.xlsx
+++ b/backend/resources/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\课程\SoftwareTesting_杜庆峰\course_project\TJ_2025Spring_SoftwareTesting_TestingTool\backend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DF0679-0466-42AC-ACD7-948516093337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB4E082-26AB-485E-B3BB-DF7324EFCCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,12 +53,6 @@
   <si>
     <t>ss</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'plot_count': 0, 'plant_plot_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1], 'plant_disease_count': {}, 'disease_count': {}, 'prediction': 'mocked_prediction'}</t>
-  </si>
-  <si>
-    <t>{'plot_count': 0, 'plant_plot_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2], 'plant_disease_count': {}, 'disease_count': {}, 'prediction': 'mocked_prediction'}</t>
   </si>
   <si>
     <t>plot_details</t>
@@ -79,28 +73,6 @@
     'logs': []
 }]</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{
-    'plotId': 'p1',
-    'plotName': '地块1',
-    'plantId': 'pl3',
-    'plantName': '植物A',
-    'plantFeature': 'feature',
-    'plantIconURL': 'icon',
-    'logs': []
-}]</t>
-  </si>
-  <si>
-    <t>[{
-    'plotId': 'p1',
-    'plotName': '地块1',
-    'plantId': 'pl4',
-    'plantName': '植物A',
-    'plantFeature': 'feature',
-    'plantIconURL': 'icon',
-    'logs': []
-}]</t>
   </si>
   <si>
     <t>list(schemas.form.PlotDetails)</t>
@@ -129,6 +101,128 @@
       </rPr>
       <t>A': 1}, 'plot_count': 1, 'prediction': 'p'}</t>
     </r>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'plot_count': 0, 'plant_plot_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0], 'plant_disease_count': {}, 'disease_count': {}, 'prediction': 'p'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试2</t>
+  </si>
+  <si>
+    <t>测试3</t>
+  </si>
+  <si>
+    <t>测试4</t>
+  </si>
+  <si>
+    <t>等价类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试5</t>
+  </si>
+  <si>
+    <t>测试6</t>
+  </si>
+  <si>
+    <t>测试7</t>
+  </si>
+  <si>
+    <t>测试8</t>
+  </si>
+  <si>
+    <t>[{
+    'plotId': '',
+    'plotName': 'plot1',
+    'plantId': 'pl2',
+    'plantName': '葡萄',
+    'plantFeature': 'feature',
+    'plantIconURL': 'icon',
+    'logs': []
+}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{
+    'plotId': 'plotId',
+    'plotName': '',
+    'plantId': 'pl2',
+    'plantName': '植物A',
+    'plantFeature': 'feature',
+    'plantIconURL': 'icon',
+    'logs': []
+}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{
+    'plotId': 'p1',
+    'plotName': '地块1',
+    'plantId': '',
+    'plantName': '植物A',
+    'plantFeature': 'feature',
+    'plantIconURL': 'icon',
+    'logs': []
+}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{
+    'plotId': 'p1',
+    'plotName': '地块1',
+    'plantId': 'pl2',
+    'plantName': '植物A',
+    'plantFeature': '',
+    'plantIconURL': 'icon',
+    'logs': []
+}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{
+    'plotId': 'p1',
+    'plotName': '地块1',
+    'plantId': 'pl2',
+    'plantName': '植物A',
+    'plantFeature': 'feature',
+    'plantIconURL': '',
+    'logs': []
+}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{'disease_count': {}, 'monthly_disease_count': [0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0], 'plant_disease_count': {}, 'plant_plot_count': {'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>葡萄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>': 1}, 'plot_count': 1, 'prediction': 'p'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -470,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -505,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.3">
@@ -513,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -525,41 +619,41 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="232.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="174.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -573,19 +667,104 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="168.5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="168.5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="168.5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="182.5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>